<commit_message>
updated splitter combiner measurement
</commit_message>
<xml_diff>
--- a/MOT-Splitter-Combiner/Splitter-Combiner-Efficiencies.xlsx
+++ b/MOT-Splitter-Combiner/Splitter-Combiner-Efficiencies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geoffreyzheng/Desktop/SrF Experiment Docs/2024 Work/3 Beam MOT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE4F573-E93C-AB48-B146-C8DBD5787AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023AD34D-F493-0D43-B570-7829C281BD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="1640" windowWidth="28040" windowHeight="17440" xr2:uid="{0BABFB9C-884C-E340-BB27-2C9953D365FB}"/>
+    <workbookView xWindow="520" yWindow="1160" windowWidth="28040" windowHeight="17440" xr2:uid="{0BABFB9C-884C-E340-BB27-2C9953D365FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="19">
   <si>
     <t>input 1</t>
   </si>
@@ -89,13 +89,10 @@
     <t>Dec 10</t>
   </si>
   <si>
-    <t>Dec 16</t>
-  </si>
-  <si>
-    <t>Dec 20</t>
-  </si>
-  <si>
     <t>Dec 23</t>
+  </si>
+  <si>
+    <t>Dec 22</t>
   </si>
 </sst>
 </file>
@@ -468,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E1A0BA-DAE7-234C-9B26-97CD695C0070}">
-  <dimension ref="A2:E87"/>
+  <dimension ref="A2:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1297,7 +1294,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B66" t="s">
         <v>5</v>
@@ -1316,30 +1313,90 @@
       <c r="A67" t="s">
         <v>0</v>
       </c>
+      <c r="B67">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="C67">
+        <v>89.7</v>
+      </c>
+      <c r="D67">
+        <v>85</v>
+      </c>
+      <c r="E67">
+        <v>86.1</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>1</v>
       </c>
+      <c r="B68">
+        <v>78</v>
+      </c>
+      <c r="C68">
+        <v>86.6</v>
+      </c>
+      <c r="D68">
+        <v>90.4</v>
+      </c>
+      <c r="E68">
+        <v>88.9</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>2</v>
       </c>
+      <c r="B69">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="C69">
+        <v>85.7</v>
+      </c>
+      <c r="D69">
+        <v>83.2</v>
+      </c>
+      <c r="E69">
+        <v>76.5</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>3</v>
       </c>
+      <c r="B70">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="C70">
+        <v>89.3</v>
+      </c>
+      <c r="D70">
+        <v>82.7</v>
+      </c>
+      <c r="E70">
+        <v>81.5</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>4</v>
       </c>
+      <c r="B71">
+        <v>83.8</v>
+      </c>
+      <c r="C71">
+        <v>88.1</v>
+      </c>
+      <c r="D71">
+        <v>89.7</v>
+      </c>
+      <c r="E71">
+        <v>88.3</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B74" t="s">
         <v>5</v>
@@ -1358,67 +1415,85 @@
       <c r="A75" t="s">
         <v>0</v>
       </c>
+      <c r="B75">
+        <v>79.2</v>
+      </c>
+      <c r="C75">
+        <v>89.8</v>
+      </c>
+      <c r="D75">
+        <v>86.9</v>
+      </c>
+      <c r="E75">
+        <v>86.9</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>1</v>
       </c>
+      <c r="B76">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="C76">
+        <v>86.2</v>
+      </c>
+      <c r="D76">
+        <v>91</v>
+      </c>
+      <c r="E76">
+        <v>90.3</v>
+      </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>2</v>
       </c>
+      <c r="B77">
+        <v>77</v>
+      </c>
+      <c r="C77">
+        <v>84.2</v>
+      </c>
+      <c r="D77">
+        <v>83.9</v>
+      </c>
+      <c r="E77">
+        <v>77.8</v>
+      </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>3</v>
       </c>
+      <c r="B78">
+        <v>73.7</v>
+      </c>
+      <c r="C78">
+        <v>89.9</v>
+      </c>
+      <c r="D78">
+        <v>83.6</v>
+      </c>
+      <c r="E78">
+        <v>80.5</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B82" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" t="s">
-        <v>7</v>
-      </c>
-      <c r="E82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>4</v>
+      <c r="B79">
+        <v>85</v>
+      </c>
+      <c r="C79">
+        <v>92.6</v>
+      </c>
+      <c r="D79">
+        <v>90.1</v>
+      </c>
+      <c r="E79">
+        <v>87.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>